<commit_message>
Auto export CCCTR-1214 - BB Security balicek
</commit_message>
<xml_diff>
--- a/exports/testcases_CCCTR-1214_-_BB_Security_balicek.xlsx
+++ b/exports/testcases_CCCTR-1214_-_BB_Security_balicek.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -582,7 +582,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -858,7 +858,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -927,7 +927,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1134,7 +1134,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2652,7 +2652,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3480,7 +3480,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3687,7 +3687,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3894,7 +3894,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4032,7 +4032,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4239,7 +4239,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4308,7 +4308,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4377,7 +4377,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4446,7 +4446,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4515,7 +4515,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4584,7 +4584,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4653,7 +4653,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -4722,7 +4722,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -4791,7 +4791,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -4998,7 +4998,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5067,7 +5067,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5136,7 +5136,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5205,7 +5205,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5274,7 +5274,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5343,7 +5343,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5412,7 +5412,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -5550,7 +5550,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -5619,7 +5619,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -5757,7 +5757,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -5826,7 +5826,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -5895,7 +5895,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -5964,7 +5964,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6033,7 +6033,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -6171,7 +6171,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6240,7 +6240,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -6378,7 +6378,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -6516,7 +6516,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -6585,7 +6585,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -6723,7 +6723,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -6861,7 +6861,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -6930,7 +6930,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -6999,7 +6999,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -7068,7 +7068,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -7137,7 +7137,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -7206,7 +7206,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -7275,7 +7275,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -7344,7 +7344,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -7413,7 +7413,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -7482,7 +7482,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -7551,7 +7551,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -7620,7 +7620,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -7689,7 +7689,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -7758,7 +7758,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -7827,7 +7827,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -7896,7 +7896,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -7965,7 +7965,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -8034,7 +8034,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -8103,7 +8103,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -8172,7 +8172,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -8241,7 +8241,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -8310,7 +8310,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -8448,7 +8448,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -8517,7 +8517,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -8586,7 +8586,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -8655,7 +8655,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -8724,7 +8724,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -8793,7 +8793,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -8862,7 +8862,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -8931,7 +8931,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -9000,7 +9000,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -9069,7 +9069,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -9138,7 +9138,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -9207,7 +9207,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -9276,7 +9276,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -9345,7 +9345,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -9414,7 +9414,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -9483,7 +9483,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -9552,7 +9552,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -9621,7 +9621,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -9690,7 +9690,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -9759,7 +9759,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -9828,7 +9828,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -9897,7 +9897,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -9966,7 +9966,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -10035,7 +10035,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -10104,7 +10104,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>UAT2\Antoso</t>
+          <t>UAT2\Antosova\2025\Converged Connectivity\NonRelease\CCCTR-1214 - BB Security balicek</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">

</xml_diff>